<commit_message>
Tests avec 2 autres photos et nouvelle formule
</commit_message>
<xml_diff>
--- a/docs/Angles photo.xlsx
+++ b/docs/Angles photo.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="23910" windowHeight="10155" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="23910" windowHeight="10155" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Formules" sheetId="1" r:id="rId1"/>
     <sheet name="Calculs Rova" sheetId="2" r:id="rId2"/>
     <sheet name="Coords" sheetId="3" r:id="rId3"/>
+    <sheet name="Radiateur" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="a">Coords!$D$16</definedName>
@@ -26,11 +27,13 @@
     <definedName name="e">Formules!$H$5</definedName>
     <definedName name="f">Formules!$C$3</definedName>
     <definedName name="h">Coords!$D$10</definedName>
+    <definedName name="lE">Radiateur!$R$5</definedName>
     <definedName name="t">Formules!$C$8</definedName>
     <definedName name="tMax">Formules!$C$4</definedName>
     <definedName name="tR">Formules!$C$9</definedName>
     <definedName name="tRTém">Formules!$C$6</definedName>
     <definedName name="tTém">Formules!$C$5</definedName>
+    <definedName name="w">Radiateur!$R$7</definedName>
     <definedName name="x">Coords!$D$18</definedName>
     <definedName name="x_1">Coords!$D$6</definedName>
     <definedName name="x_2">Coords!$D$8</definedName>
@@ -45,13 +48,145 @@
     <definedName name="y_4">Coords!$G$9</definedName>
     <definedName name="ymax">Coords!$D$14</definedName>
     <definedName name="ymin">Coords!$D$12</definedName>
+    <definedName name="αE">Radiateur!$R$4</definedName>
+    <definedName name="ρE">Radiateur!$R$6</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>LAVIGNE Mathieu (mlavigne)</author>
+  </authors>
+  <commentList>
+    <comment ref="D3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">LAVIGNE Mathieu (mlavigne):
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fonction à implémenter pour chaque objectif. alpha(l)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>LAVIGNE Mathieu (mlavigne):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Direction (google 0..360) par rapport au Nord</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>LAVIGNE Mathieu (mlavigne):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Direction du centre</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>LAVIGNE Mathieu (mlavigne):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fonction à implémenter pour chaque objectif. f(dx, dy, width, height)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K40" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>LAVIGNE Mathieu (mlavigne):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Affecter des poids à chaque calcul en fonction de l'erreur de mesure pour chaque point</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="130">
   <si>
     <t>Largeur CCD</t>
   </si>
@@ -291,18 +426,324 @@
   </si>
   <si>
     <t>Lac Anda. D top-right</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>α</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>dy</t>
+  </si>
+  <si>
+    <t>Repère :</t>
+  </si>
+  <si>
+    <r>
+      <t>α</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <t>40 ronds</t>
+  </si>
+  <si>
+    <t>80 ronds</t>
+  </si>
+  <si>
+    <t>dir</t>
+  </si>
+  <si>
+    <r>
+      <t>dir</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C</t>
+    </r>
+  </si>
+  <si>
+    <t>(- à gauche, + à droite)</t>
+  </si>
+  <si>
+    <t>(tan alpha E / l E)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ρ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <t>width =</t>
+  </si>
+  <si>
+    <t>Photo</t>
+  </si>
+  <si>
+    <t>Radiateur</t>
+  </si>
+  <si>
+    <t>Rova</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>éc. type dir</t>
+  </si>
+  <si>
+    <t>Jardin du Clos Mutta 2.JPG</t>
+  </si>
+  <si>
+    <t>Cheminée tourterelles min</t>
+  </si>
+  <si>
+    <t>Cheminée tourterelles max</t>
+  </si>
+  <si>
+    <t>Cabane gauche</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prendre à chaque repère le bord </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gauche</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>le</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>plus près</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de l'objectif</t>
+    </r>
+  </si>
+  <si>
+    <t>Papouf cheminée 1 min</t>
+  </si>
+  <si>
+    <t>Papouf cheminée 2 max</t>
+  </si>
+  <si>
+    <t>Papouf cheminée 3 max</t>
+  </si>
+  <si>
+    <t>Papouf cheminée 1 max</t>
+  </si>
+  <si>
+    <t>Papouf cheminée 2 min</t>
+  </si>
+  <si>
+    <t>Papouf cheminée 3 min</t>
+  </si>
+  <si>
+    <t>Papouf vasistas min</t>
+  </si>
+  <si>
+    <t>Papouf vasistas max</t>
+  </si>
+  <si>
+    <t>Fêt devant papouf</t>
+  </si>
+  <si>
+    <t>Compteur électrique</t>
+  </si>
+  <si>
+    <t>Cabane Patricia bord proche</t>
+  </si>
+  <si>
+    <t>Goutières tourterelles</t>
+  </si>
+  <si>
+    <t>erreur/km</t>
+  </si>
+  <si>
+    <t>distance min</t>
+  </si>
+  <si>
+    <t>distance max</t>
+  </si>
+  <si>
+    <t>erreur min</t>
+  </si>
+  <si>
+    <t>erreur max</t>
+  </si>
+  <si>
+    <t>Chéminée entre deux min</t>
+  </si>
+  <si>
+    <t>Chéminée entre deux max</t>
+  </si>
+  <si>
+    <t>Coucher de soleil sur Romillé.JPG</t>
+  </si>
+  <si>
+    <t>École cheminée 3 min</t>
+  </si>
+  <si>
+    <t>École cheminée 3 max</t>
+  </si>
+  <si>
+    <t>éc. type/km</t>
+  </si>
+  <si>
+    <t>Poteau compteur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0&quot; px&quot;"/>
     <numFmt numFmtId="166" formatCode="0.00&quot;°&quot;"/>
+    <numFmt numFmtId="167" formatCode="0.00&quot; °&quot;"/>
+    <numFmt numFmtId="170" formatCode="0&quot; m&quot;"/>
+    <numFmt numFmtId="171" formatCode="0.0&quot; m&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,8 +772,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,8 +831,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -375,12 +855,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -403,14 +894,71 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="26">
     <dxf>
       <numFmt numFmtId="165" formatCode="0&quot; px&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00&quot; °&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00&quot; °&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0&quot; px&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0&quot; px&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0&quot; px&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00&quot; °&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00&quot; °&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0&quot; px&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0&quot; px&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0&quot; px&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0&quot; px&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00&quot; °&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00&quot; °&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -443,6 +991,9 @@
       <numFmt numFmtId="165" formatCode="0&quot; px&quot;"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="165" formatCode="0&quot; px&quot;"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -453,6 +1004,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF8696B"/>
+      <color rgb="FF63BE7B"/>
       <color rgb="FFFFFF99"/>
     </mruColors>
   </colors>
@@ -574,23 +1127,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="69837952"/>
-        <c:axId val="69840256"/>
+        <c:axId val="132376832"/>
+        <c:axId val="154820608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69837952"/>
+        <c:axId val="132376832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0&quot; px&quot;" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69840256"/>
+        <c:crossAx val="154820608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69840256"/>
+        <c:axId val="154820608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -598,7 +1151,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69837952"/>
+        <c:crossAx val="132376832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -611,7 +1164,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -670,38 +1223,85 @@
   </sortState>
   <tableColumns count="13">
     <tableColumn id="11" name="Nom"/>
-    <tableColumn id="1" name="x" dataDxfId="10"/>
-    <tableColumn id="14" name="Colonne1" dataDxfId="0"/>
-    <tableColumn id="2" name="direction" dataDxfId="9"/>
-    <tableColumn id="9" name="angle théoriq." dataDxfId="8">
+    <tableColumn id="1" name="x" dataDxfId="24"/>
+    <tableColumn id="14" name="Colonne1" dataDxfId="23"/>
+    <tableColumn id="2" name="direction" dataDxfId="22"/>
+    <tableColumn id="9" name="angle théoriq." dataDxfId="21">
       <calculatedColumnFormula>Tableau1[[#This Row],[pos.]]*angle/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="dx" dataDxfId="7">
+    <tableColumn id="3" name="dx" dataDxfId="20">
       <calculatedColumnFormula>B4-960</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="pos." dataCellStyle="Pourcentage">
       <calculatedColumnFormula>Tableau1[[#This Row],[dx]]/960</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="abs(dx)" dataDxfId="6">
+    <tableColumn id="4" name="abs(dx)" dataDxfId="19">
       <calculatedColumnFormula>ABS(F4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="d. dir." dataDxfId="5">
+    <tableColumn id="5" name="d. dir." dataDxfId="18">
       <calculatedColumnFormula>Tableau1[[#This Row],[direction]]-centre_direction</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="abs(ddir)" dataDxfId="4">
+    <tableColumn id="12" name="abs(ddir)" dataDxfId="17">
       <calculatedColumnFormula>ABS(Tableau1[[#This Row],[d. dir.]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="dpx / d°" dataDxfId="3">
+    <tableColumn id="6" name="dpx / d°" dataDxfId="16">
       <calculatedColumnFormula>Tableau1[[#This Row],[dx]]/Tableau1[[#This Row],[d. dir.]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="d° / dpx %" dataDxfId="2">
+    <tableColumn id="7" name="d° / dpx %" dataDxfId="15">
       <calculatedColumnFormula>Tableau1[[#This Row],[d. dir.]]/Tableau1[[#This Row],[dx]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="correction angulaire" dataDxfId="1">
+    <tableColumn id="10" name="correction angulaire" dataDxfId="14">
       <calculatedColumnFormula>Tableau1[[#This Row],[d. dir.]]/Tableau1[[#This Row],[angle théoriq.]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B3:N40" totalsRowCount="1">
+  <autoFilter ref="B3:N39">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Coucher de soleil sur Romillé.JPG"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="1"/>
+    <filterColumn colId="8"/>
+    <filterColumn colId="9"/>
+    <filterColumn colId="12"/>
+  </autoFilter>
+  <tableColumns count="13">
+    <tableColumn id="1" name="Photo" totalsRowLabel="Total"/>
+    <tableColumn id="13" name="Nom"/>
+    <tableColumn id="2" name="α" dataDxfId="13">
+      <calculatedColumnFormula>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="dir" dataDxfId="12"/>
+    <tableColumn id="4" name="x" dataDxfId="11"/>
+    <tableColumn id="5" name="y" dataDxfId="10"/>
+    <tableColumn id="6" name="width" dataDxfId="9">
+      <calculatedColumnFormula>w</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="height" dataDxfId="8"/>
+    <tableColumn id="11" name="dirC" totalsRowFunction="average" dataDxfId="7" totalsRowDxfId="2">
+      <calculatedColumnFormula>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" name="éc. type dir" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="1">
+      <calculatedColumnFormula>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</calculatedColumnFormula>
+      <totalsRowFormula>SUBTOTAL(107,[dirC])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="8" name="dx" dataDxfId="5">
+      <calculatedColumnFormula>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="dy" dataDxfId="4">
+      <calculatedColumnFormula>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" name="l" dataDxfId="3" totalsRowDxfId="0">
+      <calculatedColumnFormula>Tableau2[[#This Row],[dx]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1320,7 +1920,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="25" priority="1">
       <formula>E19&gt;$C$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1333,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1568,7 +2168,7 @@
         <v>-23.251492226523705</v>
       </c>
       <c r="F8" s="13">
-        <f>B8-960</f>
+        <f t="shared" ref="F8:F23" si="0">B8-960</f>
         <v>-626</v>
       </c>
       <c r="G8" s="15">
@@ -1576,7 +2176,7 @@
         <v>-0.65208333333333335</v>
       </c>
       <c r="H8" s="13">
-        <f>ABS(F8)</f>
+        <f t="shared" ref="H8:H23" si="1">ABS(F8)</f>
         <v>626</v>
       </c>
       <c r="I8" s="14">
@@ -1618,7 +2218,7 @@
         <v>-23.511492938321897</v>
       </c>
       <c r="F9" s="13">
-        <f>B9-960</f>
+        <f t="shared" si="0"/>
         <v>-633</v>
       </c>
       <c r="G9" s="15">
@@ -1626,7 +2226,7 @@
         <v>-0.65937500000000004</v>
       </c>
       <c r="H9" s="13">
-        <f>ABS(F9)</f>
+        <f t="shared" si="1"/>
         <v>633</v>
       </c>
       <c r="I9" s="14">
@@ -1668,7 +2268,7 @@
         <v>-23.845779567776706</v>
       </c>
       <c r="F10" s="13">
-        <f>B10-960</f>
+        <f t="shared" si="0"/>
         <v>-642</v>
       </c>
       <c r="G10" s="15">
@@ -1676,7 +2276,7 @@
         <v>-0.66874999999999996</v>
       </c>
       <c r="H10" s="13">
-        <f>ABS(F10)</f>
+        <f t="shared" si="1"/>
         <v>642</v>
       </c>
       <c r="I10" s="14">
@@ -1716,7 +2316,7 @@
         <v>-19.797197055490631</v>
       </c>
       <c r="F11" s="13">
-        <f>B11-960</f>
+        <f t="shared" si="0"/>
         <v>-533</v>
       </c>
       <c r="G11" s="15">
@@ -1724,7 +2324,7 @@
         <v>-0.5552083333333333</v>
       </c>
       <c r="H11" s="13">
-        <f>ABS(F11)</f>
+        <f t="shared" si="1"/>
         <v>533</v>
       </c>
       <c r="I11" s="14">
@@ -1761,7 +2361,7 @@
         <v>-12.368605289828105</v>
       </c>
       <c r="F12" s="9">
-        <f>B12-960</f>
+        <f t="shared" si="0"/>
         <v>-333</v>
       </c>
       <c r="G12" s="11">
@@ -1769,7 +2369,7 @@
         <v>-0.34687499999999999</v>
       </c>
       <c r="H12" s="9">
-        <f>ABS(F12)</f>
+        <f t="shared" si="1"/>
         <v>333</v>
       </c>
       <c r="I12" s="10">
@@ -1809,7 +2409,7 @@
         <v>-10.511457348412474</v>
       </c>
       <c r="F13" s="13">
-        <f>B13-960</f>
+        <f t="shared" si="0"/>
         <v>-283</v>
       </c>
       <c r="G13" s="15">
@@ -1817,7 +2417,7 @@
         <v>-0.29479166666666667</v>
       </c>
       <c r="H13" s="13">
-        <f>ABS(F13)</f>
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="I13" s="14">
@@ -1854,7 +2454,7 @@
         <v>-7.6143065598040884</v>
       </c>
       <c r="F14" s="9">
-        <f>B14-960</f>
+        <f t="shared" si="0"/>
         <v>-205</v>
       </c>
       <c r="G14" s="11">
@@ -1862,7 +2462,7 @@
         <v>-0.21354166666666666</v>
       </c>
       <c r="H14" s="9">
-        <f>ABS(F14)</f>
+        <f t="shared" si="1"/>
         <v>205</v>
       </c>
       <c r="I14" s="10">
@@ -1902,7 +2502,7 @@
         <v>-7.3171628891775882</v>
       </c>
       <c r="F15" s="13">
-        <f>B15-960</f>
+        <f t="shared" si="0"/>
         <v>-197</v>
       </c>
       <c r="G15" s="15">
@@ -1910,7 +2510,7 @@
         <v>-0.20520833333333333</v>
       </c>
       <c r="H15" s="13">
-        <f>ABS(F15)</f>
+        <f t="shared" si="1"/>
         <v>197</v>
       </c>
       <c r="I15" s="14">
@@ -1950,7 +2550,7 @@
         <v>-6.3514459596414596</v>
       </c>
       <c r="F16" s="13">
-        <f>B16-960</f>
+        <f t="shared" si="0"/>
         <v>-171</v>
       </c>
       <c r="G16" s="15">
@@ -1958,7 +2558,7 @@
         <v>-0.17812500000000001</v>
       </c>
       <c r="H16" s="13">
-        <f>ABS(F16)</f>
+        <f t="shared" si="1"/>
         <v>171</v>
       </c>
       <c r="I16" s="14">
@@ -1995,7 +2595,7 @@
         <v>-6.1285882066715835</v>
       </c>
       <c r="F17" s="9">
-        <f>B17-960</f>
+        <f t="shared" si="0"/>
         <v>-165</v>
       </c>
       <c r="G17" s="11">
@@ -2003,7 +2603,7 @@
         <v>-0.171875</v>
       </c>
       <c r="H17" s="9">
-        <f>ABS(F17)</f>
+        <f t="shared" si="1"/>
         <v>165</v>
       </c>
       <c r="I17" s="10">
@@ -2040,7 +2640,7 @@
         <v>7.6143065598040884</v>
       </c>
       <c r="F18" s="9">
-        <f>B18-960</f>
+        <f t="shared" si="0"/>
         <v>205</v>
       </c>
       <c r="G18" s="11">
@@ -2048,7 +2648,7 @@
         <v>0.21354166666666666</v>
       </c>
       <c r="H18" s="9">
-        <f>ABS(F18)</f>
+        <f t="shared" si="1"/>
         <v>205</v>
       </c>
       <c r="I18" s="10">
@@ -2085,7 +2685,7 @@
         <v>10.511457348412474</v>
       </c>
       <c r="F19" s="9">
-        <f>B19-960</f>
+        <f t="shared" si="0"/>
         <v>283</v>
       </c>
       <c r="G19" s="11">
@@ -2093,7 +2693,7 @@
         <v>0.29479166666666667</v>
       </c>
       <c r="H19" s="9">
-        <f>ABS(F19)</f>
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="I19" s="10">
@@ -2130,7 +2730,7 @@
         <v>11.180030607322101</v>
       </c>
       <c r="F20" s="9">
-        <f>B20-960</f>
+        <f t="shared" si="0"/>
         <v>301</v>
       </c>
       <c r="G20" s="11">
@@ -2138,7 +2738,7 @@
         <v>0.31354166666666666</v>
       </c>
       <c r="H20" s="9">
-        <f>ABS(F20)</f>
+        <f t="shared" si="1"/>
         <v>301</v>
       </c>
       <c r="I20" s="10">
@@ -2178,7 +2778,7 @@
         <v>24.700067620827902</v>
       </c>
       <c r="F21" s="13">
-        <f>B21-960</f>
+        <f t="shared" si="0"/>
         <v>665</v>
       </c>
       <c r="G21" s="15">
@@ -2186,7 +2786,7 @@
         <v>0.69270833333333337</v>
       </c>
       <c r="H21" s="13">
-        <f>ABS(F21)</f>
+        <f t="shared" si="1"/>
         <v>665</v>
       </c>
       <c r="I21" s="14">
@@ -2226,7 +2826,7 @@
         <v>32.982947439541618</v>
       </c>
       <c r="F22" s="13">
-        <f>B22-960</f>
+        <f t="shared" si="0"/>
         <v>888</v>
       </c>
       <c r="G22" s="15">
@@ -2234,7 +2834,7 @@
         <v>0.92500000000000004</v>
       </c>
       <c r="H22" s="13">
-        <f>ABS(F22)</f>
+        <f t="shared" si="1"/>
         <v>888</v>
       </c>
       <c r="I22" s="14">
@@ -2274,7 +2874,7 @@
         <v>34.097236204390995</v>
       </c>
       <c r="F23" s="13">
-        <f>B23-960</f>
+        <f t="shared" si="0"/>
         <v>918</v>
       </c>
       <c r="G23" s="15">
@@ -2282,7 +2882,7 @@
         <v>0.95625000000000004</v>
       </c>
       <c r="H23" s="13">
-        <f>ABS(F23)</f>
+        <f t="shared" si="1"/>
         <v>918</v>
       </c>
       <c r="I23" s="14">
@@ -2320,7 +2920,7 @@
   <dimension ref="B4:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2545,4 +3145,1863 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:S45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="3" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="16" max="16" width="3.28515625" customWidth="1"/>
+    <col min="17" max="17" width="4.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:19">
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="26">
+        <f>DEGREES(ATAN(N1*ρE))</f>
+        <v>8.8550638195003852</v>
+      </c>
+      <c r="E1" s="25">
+        <f>Tableau2[[#Totals],[dirC]]+D1</f>
+        <v>217.79889491614171</v>
+      </c>
+      <c r="F1" s="31">
+        <v>1187</v>
+      </c>
+      <c r="H1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="37">
+        <f>1000*TAN(RADIANS(E1-E2))</f>
+        <v>565.51694431664316</v>
+      </c>
+      <c r="J1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" s="35">
+        <v>1000</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="M1" s="34">
+        <f>$K1*TAN(RADIANS($E$1-$E$2))</f>
+        <v>565.51694431664316</v>
+      </c>
+      <c r="N1" s="9">
+        <f>F1-w/2</f>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="2:19">
+      <c r="D2" s="26">
+        <f>E2-Tableau2[[#Totals],[dirC]]</f>
+        <v>-20.63383109664133</v>
+      </c>
+      <c r="E2" s="32">
+        <v>188.31</v>
+      </c>
+      <c r="F2" s="36">
+        <f>TAN(RADIANS($E$2-Tableau2[[#Totals],[dirC]]))/ρE+w/2</f>
+        <v>411.34233014594531</v>
+      </c>
+      <c r="H2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" s="37">
+        <f>1000*TAN(RADIANS(Tableau2[[#Totals],[éc. type dir]]))</f>
+        <v>37.173273445494821</v>
+      </c>
+      <c r="J2" t="s">
+        <v>120</v>
+      </c>
+      <c r="K2" s="37">
+        <v>2000</v>
+      </c>
+      <c r="L2" t="s">
+        <v>122</v>
+      </c>
+      <c r="M2" s="34">
+        <f>$K2*TAN(RADIANS($E$1-$E$2))</f>
+        <v>1131.0338886332863</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" ht="18">
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" ht="18" hidden="1" customHeight="1">
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="25">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-31.13</v>
+      </c>
+      <c r="E4" s="25">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
+        <v>80</v>
+      </c>
+      <c r="G4" s="9">
+        <v>540</v>
+      </c>
+      <c r="H4" s="9">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I4" s="9">
+        <v>1080</v>
+      </c>
+      <c r="J4" s="25">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>31.13</v>
+      </c>
+      <c r="K4" s="25">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-177.81383109664134</v>
+      </c>
+      <c r="L4" s="9">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-880</v>
+      </c>
+      <c r="M4" s="9">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="9">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-880</v>
+      </c>
+      <c r="Q4" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="R4" s="27">
+        <v>-31.13</v>
+      </c>
+      <c r="S4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" ht="18" hidden="1" customHeight="1">
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="25">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-16.803080314749245</v>
+      </c>
+      <c r="E5" s="25">
+        <v>14.33</v>
+      </c>
+      <c r="F5" s="9">
+        <v>520</v>
+      </c>
+      <c r="G5" s="9">
+        <v>540</v>
+      </c>
+      <c r="H5" s="9">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I5" s="9">
+        <v>1080</v>
+      </c>
+      <c r="J5" s="25">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>31.133080314749243</v>
+      </c>
+      <c r="K5" s="25">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-177.8107507818921</v>
+      </c>
+      <c r="L5" s="9">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-440</v>
+      </c>
+      <c r="M5" s="9">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="9">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-440</v>
+      </c>
+      <c r="Q5" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="R5" s="28">
+        <v>-880</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" ht="18" hidden="1">
+      <c r="B6" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-25.979057450062179</v>
+      </c>
+      <c r="E6" s="30">
+        <v>272.71891597241103</v>
+      </c>
+      <c r="F6" s="13">
+        <v>250</v>
+      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>298.69797342247318</v>
+      </c>
+      <c r="K6" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>89.75414232583185</v>
+      </c>
+      <c r="L6" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-710</v>
+      </c>
+      <c r="M6" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-710</v>
+      </c>
+      <c r="Q6" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="R6" s="29">
+        <f>TAN(RADIANS(αE))/lE</f>
+        <v>6.8631014445932035E-4</v>
+      </c>
+      <c r="S6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" hidden="1">
+      <c r="B7" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-25.979057450062179</v>
+      </c>
+      <c r="E7" s="30">
+        <v>273.20320836215097</v>
+      </c>
+      <c r="F7" s="13">
+        <v>250</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I7" s="13"/>
+      <c r="J7" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>299.18226581221313</v>
+      </c>
+      <c r="K7" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>90.238434715571799</v>
+      </c>
+      <c r="L7" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-710</v>
+      </c>
+      <c r="M7" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-710</v>
+      </c>
+      <c r="Q7" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="R7" s="28">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" hidden="1">
+      <c r="B8" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-23.481780707111938</v>
+      </c>
+      <c r="E8" s="30">
+        <v>275.26357220511602</v>
+      </c>
+      <c r="F8" s="13">
+        <v>327</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I8" s="13"/>
+      <c r="J8" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>298.74535291222799</v>
+      </c>
+      <c r="K8" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>89.801521815586653</v>
+      </c>
+      <c r="L8" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-633</v>
+      </c>
+      <c r="M8" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-633</v>
+      </c>
+      <c r="Q8" s="24"/>
+    </row>
+    <row r="9" spans="2:19" hidden="1">
+      <c r="B9" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-23.778822820475099</v>
+      </c>
+      <c r="E9" s="30">
+        <v>275.75532567420402</v>
+      </c>
+      <c r="F9" s="13">
+        <v>318</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I9" s="13"/>
+      <c r="J9" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>299.53414849467913</v>
+      </c>
+      <c r="K9" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>90.590317398037797</v>
+      </c>
+      <c r="L9" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-642</v>
+      </c>
+      <c r="M9" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-642</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" hidden="1">
+      <c r="B10" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-20.092686780924236</v>
+      </c>
+      <c r="E10" s="30">
+        <v>278.66000000000003</v>
+      </c>
+      <c r="F10" s="13">
+        <v>427</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>298.75268678092425</v>
+      </c>
+      <c r="K10" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>89.808855684282918</v>
+      </c>
+      <c r="L10" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-533</v>
+      </c>
+      <c r="M10" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-533</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" hidden="1">
+      <c r="B11" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-10.991467734534149</v>
+      </c>
+      <c r="E11" s="30">
+        <v>288.94</v>
+      </c>
+      <c r="F11" s="13">
+        <v>677</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I11" s="13"/>
+      <c r="J11" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>299.93146773453412</v>
+      </c>
+      <c r="K11" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>90.987636637892791</v>
+      </c>
+      <c r="L11" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-283</v>
+      </c>
+      <c r="M11" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-283</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" hidden="1">
+      <c r="B12" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-7.6998758638936255</v>
+      </c>
+      <c r="E12" s="30">
+        <v>292.24</v>
+      </c>
+      <c r="F12" s="13">
+        <v>763</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I12" s="13"/>
+      <c r="J12" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>299.93987586389363</v>
+      </c>
+      <c r="K12" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>90.9960447672523</v>
+      </c>
+      <c r="L12" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-197</v>
+      </c>
+      <c r="M12" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-197</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" hidden="1">
+      <c r="B13" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-6.6935589886281344</v>
+      </c>
+      <c r="E13" s="30">
+        <v>293.20999999999998</v>
+      </c>
+      <c r="F13" s="13">
+        <v>789</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I13" s="13"/>
+      <c r="J13" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>299.90355898862811</v>
+      </c>
+      <c r="K13" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>90.959727891986773</v>
+      </c>
+      <c r="L13" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-171</v>
+      </c>
+      <c r="M13" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-171</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" hidden="1">
+      <c r="B14" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>3.4561971895655663</v>
+      </c>
+      <c r="E14" s="30">
+        <v>183.95</v>
+      </c>
+      <c r="F14" s="13">
+        <v>1048</v>
+      </c>
+      <c r="G14" s="13">
+        <v>82</v>
+      </c>
+      <c r="H14" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I14" s="13"/>
+      <c r="J14" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>180.49380281043443</v>
+      </c>
+      <c r="K14" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-28.450028286206901</v>
+      </c>
+      <c r="L14" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>88</v>
+      </c>
+      <c r="M14" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>82</v>
+      </c>
+      <c r="N14" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" hidden="1">
+      <c r="B15" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>4.6299713615815881</v>
+      </c>
+      <c r="E15" s="30">
+        <v>183.95</v>
+      </c>
+      <c r="F15" s="13">
+        <v>1078</v>
+      </c>
+      <c r="G15" s="13">
+        <v>87</v>
+      </c>
+      <c r="H15" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I15" s="13"/>
+      <c r="J15" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>179.32002863841839</v>
+      </c>
+      <c r="K15" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-29.62380245822294</v>
+      </c>
+      <c r="L15" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>118</v>
+      </c>
+      <c r="M15" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>87</v>
+      </c>
+      <c r="N15" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" hidden="1">
+      <c r="B16" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-7.4293879789011283</v>
+      </c>
+      <c r="E16" s="30">
+        <v>170.58</v>
+      </c>
+      <c r="F16" s="13">
+        <v>770</v>
+      </c>
+      <c r="G16" s="13">
+        <v>235</v>
+      </c>
+      <c r="H16" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I16" s="13"/>
+      <c r="J16" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>178.00938797890115</v>
+      </c>
+      <c r="K16" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-30.934443117740187</v>
+      </c>
+      <c r="L16" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-190</v>
+      </c>
+      <c r="M16" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>235</v>
+      </c>
+      <c r="N16" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-190</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" hidden="1">
+      <c r="B17" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-28.161119116223961</v>
+      </c>
+      <c r="E17" s="30">
+        <v>146.79</v>
+      </c>
+      <c r="F17" s="13">
+        <v>180</v>
+      </c>
+      <c r="G17" s="13">
+        <v>356</v>
+      </c>
+      <c r="H17" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I17" s="13"/>
+      <c r="J17" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>174.95111911622396</v>
+      </c>
+      <c r="K17" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-33.992711980417369</v>
+      </c>
+      <c r="L17" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-780</v>
+      </c>
+      <c r="M17" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>356</v>
+      </c>
+      <c r="N17" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-780</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" hidden="1">
+      <c r="B18" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>12.386608410608488</v>
+      </c>
+      <c r="E18" s="30">
+        <v>191.96</v>
+      </c>
+      <c r="F18" s="13">
+        <v>1280</v>
+      </c>
+      <c r="G18" s="13">
+        <v>134</v>
+      </c>
+      <c r="H18" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I18" s="13"/>
+      <c r="J18" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>179.57339158939152</v>
+      </c>
+      <c r="K18" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-29.370439507249813</v>
+      </c>
+      <c r="L18" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>320</v>
+      </c>
+      <c r="M18" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>134</v>
+      </c>
+      <c r="N18" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" hidden="1">
+      <c r="B19" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>13.134680644883922</v>
+      </c>
+      <c r="E19" s="30">
+        <v>193.26</v>
+      </c>
+      <c r="F19" s="13">
+        <v>1300</v>
+      </c>
+      <c r="G19" s="13">
+        <v>104</v>
+      </c>
+      <c r="H19" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I19" s="13"/>
+      <c r="J19" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>180.12531935511606</v>
+      </c>
+      <c r="K19" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-28.818511741525271</v>
+      </c>
+      <c r="L19" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>340</v>
+      </c>
+      <c r="M19" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>104</v>
+      </c>
+      <c r="N19" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" hidden="1">
+      <c r="B20" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>18.410559023085899</v>
+      </c>
+      <c r="E20" s="30">
+        <v>198.26</v>
+      </c>
+      <c r="F20" s="13">
+        <v>1445</v>
+      </c>
+      <c r="G20" s="13">
+        <v>115</v>
+      </c>
+      <c r="H20" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I20" s="13"/>
+      <c r="J20" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>179.84944097691408</v>
+      </c>
+      <c r="K20" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-29.094390119727251</v>
+      </c>
+      <c r="L20" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>485</v>
+      </c>
+      <c r="M20" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>115</v>
+      </c>
+      <c r="N20" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>485</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" hidden="1">
+      <c r="B21" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>19.430977485436763</v>
+      </c>
+      <c r="E21" s="30">
+        <v>199.64</v>
+      </c>
+      <c r="F21" s="13">
+        <v>1474</v>
+      </c>
+      <c r="G21" s="13">
+        <v>113</v>
+      </c>
+      <c r="H21" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I21" s="13"/>
+      <c r="J21" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>180.20902251456323</v>
+      </c>
+      <c r="K21" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-28.734808582078102</v>
+      </c>
+      <c r="L21" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>514</v>
+      </c>
+      <c r="M21" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>113</v>
+      </c>
+      <c r="N21" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>514</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" hidden="1">
+      <c r="B22" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>24.434070558685622</v>
+      </c>
+      <c r="E22" s="30">
+        <v>204.85</v>
+      </c>
+      <c r="F22" s="13">
+        <v>1622</v>
+      </c>
+      <c r="G22" s="13">
+        <v>130</v>
+      </c>
+      <c r="H22" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I22" s="13"/>
+      <c r="J22" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>180.41592944131438</v>
+      </c>
+      <c r="K22" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-28.527901655326957</v>
+      </c>
+      <c r="L22" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>662</v>
+      </c>
+      <c r="M22" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>130</v>
+      </c>
+      <c r="N22" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>662</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" hidden="1">
+      <c r="B23" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D23" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>25.724289199762989</v>
+      </c>
+      <c r="E23" s="30">
+        <v>206.23</v>
+      </c>
+      <c r="F23" s="13">
+        <v>1662</v>
+      </c>
+      <c r="G23" s="13">
+        <v>120</v>
+      </c>
+      <c r="H23" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I23" s="13"/>
+      <c r="J23" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>180.50571080023701</v>
+      </c>
+      <c r="K23" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-28.438120296404321</v>
+      </c>
+      <c r="L23" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>702</v>
+      </c>
+      <c r="M23" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>120</v>
+      </c>
+      <c r="N23" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>702</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" hidden="1">
+      <c r="B24" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>28.76890439060919</v>
+      </c>
+      <c r="E24" s="30">
+        <v>209.99</v>
+      </c>
+      <c r="F24" s="13">
+        <v>1760</v>
+      </c>
+      <c r="G24" s="13">
+        <v>268</v>
+      </c>
+      <c r="H24" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I24" s="13"/>
+      <c r="J24" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>181.22109560939083</v>
+      </c>
+      <c r="K24" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-27.722735487250503</v>
+      </c>
+      <c r="L24" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>800</v>
+      </c>
+      <c r="M24" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>268</v>
+      </c>
+      <c r="N24" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" hidden="1">
+      <c r="B25" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>29.726800751575002</v>
+      </c>
+      <c r="E25" s="30">
+        <v>209.99</v>
+      </c>
+      <c r="F25" s="13">
+        <v>1792</v>
+      </c>
+      <c r="G25" s="13">
+        <v>284</v>
+      </c>
+      <c r="H25" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I25" s="13"/>
+      <c r="J25" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>180.263199248425</v>
+      </c>
+      <c r="K25" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-28.680631848216336</v>
+      </c>
+      <c r="L25" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>832</v>
+      </c>
+      <c r="M25" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>284</v>
+      </c>
+      <c r="N25" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>832</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" hidden="1">
+      <c r="B26" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>26.137729575063418</v>
+      </c>
+      <c r="E26" s="30">
+        <v>207.45</v>
+      </c>
+      <c r="F26" s="13">
+        <v>1675</v>
+      </c>
+      <c r="G26" s="13">
+        <v>283</v>
+      </c>
+      <c r="H26" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I26" s="13"/>
+      <c r="J26" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>181.31227042493657</v>
+      </c>
+      <c r="K26" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-27.631560671704761</v>
+      </c>
+      <c r="L26" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>715</v>
+      </c>
+      <c r="M26" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>283</v>
+      </c>
+      <c r="N26" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>715</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" hidden="1">
+      <c r="B27" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>32.268532860569394</v>
+      </c>
+      <c r="E27" s="30">
+        <v>214.08</v>
+      </c>
+      <c r="F27" s="13">
+        <v>1880</v>
+      </c>
+      <c r="G27" s="13">
+        <v>533</v>
+      </c>
+      <c r="H27" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I27" s="13"/>
+      <c r="J27" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>181.81146713943062</v>
+      </c>
+      <c r="K27" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-27.132363957210714</v>
+      </c>
+      <c r="L27" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>920</v>
+      </c>
+      <c r="M27" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>533</v>
+      </c>
+      <c r="N27" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>920</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" hidden="1">
+      <c r="B28" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>11.558754183846105</v>
+      </c>
+      <c r="E28" s="30">
+        <v>191.29</v>
+      </c>
+      <c r="F28" s="13">
+        <v>1258</v>
+      </c>
+      <c r="G28" s="13">
+        <v>202</v>
+      </c>
+      <c r="H28" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I28" s="13"/>
+      <c r="J28" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>179.73124581615389</v>
+      </c>
+      <c r="K28" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-29.212585280487446</v>
+      </c>
+      <c r="L28" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>298</v>
+      </c>
+      <c r="M28" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>202</v>
+      </c>
+      <c r="N28" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>298</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14">
+      <c r="B29" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-28.91975776201145</v>
+      </c>
+      <c r="E29" s="30">
+        <v>177.15</v>
+      </c>
+      <c r="F29" s="13">
+        <v>155</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I29" s="13"/>
+      <c r="J29" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>206.06975776201145</v>
+      </c>
+      <c r="K29" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-2.8740733346298839</v>
+      </c>
+      <c r="L29" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-805</v>
+      </c>
+      <c r="M29" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-805</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14">
+      <c r="B30" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-27.793095377280505</v>
+      </c>
+      <c r="E30" s="30">
+        <v>178.34</v>
+      </c>
+      <c r="F30" s="13">
+        <v>192</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I30" s="13"/>
+      <c r="J30" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>206.13309537728051</v>
+      </c>
+      <c r="K30" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-2.8107357193608209</v>
+      </c>
+      <c r="L30" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-768</v>
+      </c>
+      <c r="M30" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-768</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14">
+      <c r="B31" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D31" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-20.231291060007493</v>
+      </c>
+      <c r="E31" s="30">
+        <v>188.31</v>
+      </c>
+      <c r="F31" s="13">
+        <v>423</v>
+      </c>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I31" s="13"/>
+      <c r="J31" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>208.5412910600075</v>
+      </c>
+      <c r="K31" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-0.40254003663383742</v>
+      </c>
+      <c r="L31" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-537</v>
+      </c>
+      <c r="M31" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-537</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14">
+      <c r="B32" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-19.535822145647803</v>
+      </c>
+      <c r="E32" s="30">
+        <v>189.42</v>
+      </c>
+      <c r="F32" s="13">
+        <v>443</v>
+      </c>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I32" s="13"/>
+      <c r="J32" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>208.9558221456478</v>
+      </c>
+      <c r="K32" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>1.1991049006468302E-2</v>
+      </c>
+      <c r="L32" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-517</v>
+      </c>
+      <c r="M32" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-517</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14">
+      <c r="B33" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-14.248229547142955</v>
+      </c>
+      <c r="E33" s="30">
+        <v>195.08</v>
+      </c>
+      <c r="F33" s="13">
+        <v>590</v>
+      </c>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I33" s="13"/>
+      <c r="J33" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>209.32822954714297</v>
+      </c>
+      <c r="K33" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>0.38439845050163512</v>
+      </c>
+      <c r="L33" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-370</v>
+      </c>
+      <c r="M33" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-370</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14">
+      <c r="B34" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-13.395446418619677</v>
+      </c>
+      <c r="E34" s="30">
+        <v>196.03</v>
+      </c>
+      <c r="F34" s="13">
+        <v>613</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I34" s="13"/>
+      <c r="J34" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>209.42544641861969</v>
+      </c>
+      <c r="K34" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>0.48161532197835299</v>
+      </c>
+      <c r="L34" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-347</v>
+      </c>
+      <c r="M34" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N34" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-347</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14">
+      <c r="B35" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-8.2012870053680356</v>
+      </c>
+      <c r="E35" s="30">
+        <v>201.65</v>
+      </c>
+      <c r="F35" s="13">
+        <v>750</v>
+      </c>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I35" s="13"/>
+      <c r="J35" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>209.85128700536805</v>
+      </c>
+      <c r="K35" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>0.90745590872671755</v>
+      </c>
+      <c r="L35" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-210</v>
+      </c>
+      <c r="M35" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-210</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14">
+      <c r="B36" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>-7.0424011584949886</v>
+      </c>
+      <c r="E36" s="30">
+        <v>202.84</v>
+      </c>
+      <c r="F36" s="13">
+        <v>780</v>
+      </c>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I36" s="13"/>
+      <c r="J36" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>209.88240115849499</v>
+      </c>
+      <c r="K36" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>0.93857006185365321</v>
+      </c>
+      <c r="L36" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>-180</v>
+      </c>
+      <c r="M36" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N36" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>-180</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14">
+      <c r="B37" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D37" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>24.107284969136543</v>
+      </c>
+      <c r="E37" s="30">
+        <v>235.85</v>
+      </c>
+      <c r="F37" s="13">
+        <v>1612</v>
+      </c>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I37" s="13"/>
+      <c r="J37" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>211.74271503086345</v>
+      </c>
+      <c r="K37" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>2.7988839342221183</v>
+      </c>
+      <c r="L37" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>652</v>
+      </c>
+      <c r="M37" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N37" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>652</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14">
+      <c r="B38" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>25.788084157397375</v>
+      </c>
+      <c r="E38" s="30">
+        <v>238.09</v>
+      </c>
+      <c r="F38" s="13">
+        <v>1664</v>
+      </c>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I38" s="13"/>
+      <c r="J38" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>212.30191584260263</v>
+      </c>
+      <c r="K38" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>3.3580847459612926</v>
+      </c>
+      <c r="L38" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>704</v>
+      </c>
+      <c r="M38" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N38" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>704</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14">
+      <c r="B39" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" t="s">
+        <v>129</v>
+      </c>
+      <c r="D39" s="30">
+        <f>DEGREES(ATAN(Tableau2[[#This Row],[l]]*ρE))</f>
+        <v>0.58981928498443648</v>
+      </c>
+      <c r="E39" s="30">
+        <v>206.74</v>
+      </c>
+      <c r="F39" s="13">
+        <v>975</v>
+      </c>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13">
+        <f>w</f>
+        <v>1920</v>
+      </c>
+      <c r="I39" s="13"/>
+      <c r="J39" s="30">
+        <f>Tableau2[[#This Row],[dir]]-Tableau2[[#This Row],[α]]</f>
+        <v>206.15018071501558</v>
+      </c>
+      <c r="K39" s="30">
+        <f>Tableau2[[#This Row],[dirC]]-Tableau2[[#Totals],[dirC]]</f>
+        <v>-2.7936503816257527</v>
+      </c>
+      <c r="L39" s="13">
+        <f>Tableau2[[#This Row],[x]]-Tableau2[[#This Row],[width]]/2</f>
+        <v>15</v>
+      </c>
+      <c r="M39" s="13">
+        <f>Tableau2[[#This Row],[y]]-Tableau2[[#This Row],[height]]/2</f>
+        <v>0</v>
+      </c>
+      <c r="N39" s="13">
+        <f>Tableau2[[#This Row],[dx]]</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14">
+      <c r="B40" t="s">
+        <v>99</v>
+      </c>
+      <c r="J40" s="25">
+        <f>SUBTOTAL(101,[dirC])</f>
+        <v>208.94383109664133</v>
+      </c>
+      <c r="K40" s="25">
+        <f>SUBTOTAL(107,[dirC])</f>
+        <v>2.1288914357184496</v>
+      </c>
+      <c r="N40" s="9"/>
+    </row>
+    <row r="42" spans="2:14">
+      <c r="B42" t="s">
+        <v>123</v>
+      </c>
+      <c r="F42">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14">
+      <c r="B43" t="s">
+        <v>124</v>
+      </c>
+      <c r="F43">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14">
+      <c r="G44" s="25"/>
+    </row>
+    <row r="45" spans="2:14">
+      <c r="E45" s="25"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="K4:K39">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="-$K$40*2"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="$K$40*2"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="4">
+    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="H4:H39">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="I4:I39"/>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E4:E39">
+      <formula1>0</formula1>
+      <formula2>360</formula2>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F39">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>